<commit_message>
Memindahkan file keluar dari folder modul
</commit_message>
<xml_diff>
--- a/Absensi_Karyawan.xlsx
+++ b/Absensi_Karyawan.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,7 +478,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>17:02:37</t>
+          <t>19:09:55</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -490,12 +490,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Aisyah Dewani Putri</t>
+          <t>Dinnar Ary Nastiti</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>MJM001</t>
+          <t>MJM005</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -505,37 +505,10 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>17:24:02</t>
+          <t>19:15:25</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
-        <is>
-          <t>Alfa</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Fadzli Fiyannuba</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>MJM006</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>08-12-2024</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>17:32:47</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
         <is>
           <t>Alfa</t>
         </is>

</xml_diff>